<commit_message>
Zeitabrechnung, Sprint Report and small change in README.md
</commit_message>
<xml_diff>
--- a/doc/Zeitabrechnung.xlsx
+++ b/doc/Zeitabrechnung.xlsx
@@ -89,7 +89,8 @@
     <font>
       <b val="true"/>
       <i val="true"/>
-      <sz val="16"/>
+      <u val="single"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -97,9 +98,7 @@
     </font>
     <font>
       <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -115,7 +114,8 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
+      <i val="true"/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -153,7 +153,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,15 +177,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -202,11 +198,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -239,16 +235,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading1" xfId="20"/>
-    <cellStyle name="Result2" xfId="21"/>
-    <cellStyle name="Heading" xfId="22"/>
+    <cellStyle name="Ergebnis 2" xfId="20"/>
+    <cellStyle name="Heading 3" xfId="21"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -260,16 +255,16 @@
   </sheetPr>
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,7 +714,9 @@
         <v>44534</v>
       </c>
       <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+      <c r="C50" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="D50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,7 +766,9 @@
         <v>44539</v>
       </c>
       <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
+      <c r="C55" s="6" t="n">
+        <v>1.5</v>
+      </c>
       <c r="D55" s="6" t="n">
         <v>1.75</v>
       </c>
@@ -811,7 +810,9 @@
       <c r="B59" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C59" s="6"/>
+      <c r="C59" s="6" t="n">
+        <v>3</v>
+      </c>
       <c r="D59" s="6" t="n">
         <v>5.25</v>
       </c>
@@ -823,7 +824,9 @@
       <c r="B60" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C60" s="6"/>
+      <c r="C60" s="6" t="n">
+        <v>4.5</v>
+      </c>
       <c r="D60" s="6" t="n">
         <v>3</v>
       </c>
@@ -845,7 +848,9 @@
       <c r="B62" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C62" s="6"/>
+      <c r="C62" s="6" t="n">
+        <v>4</v>
+      </c>
       <c r="D62" s="6" t="n">
         <v>2</v>
       </c>
@@ -857,7 +862,9 @@
       <c r="B63" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C63" s="6"/>
+      <c r="C63" s="6" t="n">
+        <v>1.5</v>
+      </c>
       <c r="D63" s="6" t="n">
         <v>2.5</v>
       </c>
@@ -881,7 +888,9 @@
       <c r="B65" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="C65" s="6"/>
+      <c r="C65" s="6" t="n">
+        <v>9</v>
+      </c>
       <c r="D65" s="6" t="n">
         <v>6</v>
       </c>
@@ -1409,7 +1418,7 @@
       </c>
       <c r="C139" s="11" t="n">
         <f aca="false">SUM(C5:C136)</f>
-        <v>9</v>
+        <v>33.5</v>
       </c>
       <c r="D139" s="11" t="n">
         <f aca="false">SUM(D5:D136)</f>
@@ -1418,13 +1427,13 @@
       <c r="E139" s="11"/>
       <c r="F139" s="11" t="n">
         <f aca="false">SUM(B139:D139)</f>
-        <v>99.9</v>
+        <v>124.4</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fixed sass build issue
</commit_message>
<xml_diff>
--- a/doc/Zeitabrechnung.xlsx
+++ b/doc/Zeitabrechnung.xlsx
@@ -1,17 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Documents\git\project10-icconsult\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2E67FE-5A79-4307-BDC8-5C445F828FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Zeitabrechnung" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Zeitabrechnung" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -22,48 +34,47 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
-    <t xml:space="preserve">Zeitabrechnung SoPra Entwickler-Team</t>
+    <t>Zeitabrechnung SoPra Entwickler-Team</t>
   </si>
   <si>
-    <t xml:space="preserve">ID:</t>
+    <t>ID:</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
+    <t>Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruben Werbke</t>
+    <t>Ruben Werbke</t>
   </si>
   <si>
-    <t xml:space="preserve">Yichi Zhang</t>
+    <t>Yichi Zhang</t>
   </si>
   <si>
-    <t xml:space="preserve">Robin Klaß</t>
+    <t>Robin Klaß</t>
   </si>
   <si>
-    <t xml:space="preserve">Datum</t>
+    <t>Datum</t>
   </si>
   <si>
-    <t xml:space="preserve">Stundenanzahl</t>
+    <t>Stundenanzahl</t>
   </si>
   <si>
-    <t xml:space="preserve">Gesamt</t>
+    <t>Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">Summierte Stunden</t>
+    <t>Summierte Stunden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
-    <numFmt numFmtId="166" formatCode="dddd&quot;, &quot;yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="hh\:mm"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-407];[Red]\-#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="165" formatCode="dddd&quot;, &quot;yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="hh\:mm"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -72,24 +83,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
+      <b/>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -97,7 +93,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -105,7 +101,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -113,8 +109,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
+      <b/>
+      <i/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -122,7 +118,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -145,7 +141,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -153,130 +149,373 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Ergebnis 2" xfId="20"/>
-    <cellStyle name="Heading 3" xfId="21"/>
+  <cellStyles count="3">
+    <cellStyle name="Ergebnis 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Heading 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.61"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="4" width="13.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.875" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -287,7 +526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -298,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -312,56 +551,56 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>44489</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>44490</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>44491</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>44492</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>44493</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>44494</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>44495</v>
       </c>
       <c r="B11" s="6"/>
@@ -369,1072 +608,1107 @@
       <c r="D11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>44496</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>44497</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>44498</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>44499</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>44500</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>44501</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>44502</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>44503</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>44504</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>44505</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>44506</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>44507</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>44508</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>44509</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>44510</v>
       </c>
-      <c r="B26" s="6" t="n">
+      <c r="B26" s="6">
         <v>1</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>44511</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>44512</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>44513</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>44514</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="6" t="n">
+      <c r="D30" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>44515</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>44516</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="6" t="n">
+      <c r="D32" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>44517</v>
       </c>
-      <c r="B33" s="6" t="n">
+      <c r="B33" s="6">
         <v>1</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>44518</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>44519</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="6" t="n">
+      <c r="C35" s="6">
         <v>3.5</v>
       </c>
-      <c r="D35" s="6" t="n">
+      <c r="D35" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>44520</v>
       </c>
-      <c r="B36" s="6" t="n">
+      <c r="B36" s="6">
         <v>2.5</v>
       </c>
-      <c r="C36" s="6" t="n">
+      <c r="C36" s="6">
         <v>2.5</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D36" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>44521</v>
       </c>
-      <c r="B37" s="6" t="n">
+      <c r="B37" s="6">
         <v>2.4</v>
       </c>
-      <c r="C37" s="6" t="n">
+      <c r="C37" s="6">
         <v>3</v>
       </c>
-      <c r="D37" s="6" t="n">
+      <c r="D37" s="6">
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>44522</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="6" t="n">
+      <c r="D38" s="6">
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>44523</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>44524</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>44525</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>44526</v>
       </c>
-      <c r="B42" s="6" t="n">
+      <c r="B42" s="6">
         <v>1.5</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>44527</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>44528</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="6" t="n">
+      <c r="D44" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>44529</v>
       </c>
-      <c r="B45" s="6" t="n">
+      <c r="B45" s="6">
         <v>4</v>
       </c>
       <c r="C45" s="6"/>
-      <c r="D45" s="6" t="n">
+      <c r="D45" s="6">
         <v>2.5</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>44530</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="6" t="n">
+      <c r="D46" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>44531</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>44532</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>44533</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>44534</v>
       </c>
       <c r="B50" s="6"/>
-      <c r="C50" s="6" t="n">
+      <c r="C50" s="6">
         <v>1</v>
       </c>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>44535</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
-      <c r="D51" s="6" t="n">
+      <c r="D51" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>44536</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="6" t="n">
+      <c r="D52" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>44537</v>
       </c>
-      <c r="B53" s="6" t="n">
+      <c r="B53" s="6">
         <v>2</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>44538</v>
       </c>
-      <c r="B54" s="6" t="n">
+      <c r="B54" s="6">
         <v>1</v>
       </c>
       <c r="C54" s="6"/>
-      <c r="D54" s="6" t="n">
+      <c r="D54" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>44539</v>
       </c>
       <c r="B55" s="6"/>
-      <c r="C55" s="6" t="n">
+      <c r="C55" s="6">
         <v>1.5</v>
       </c>
-      <c r="D55" s="6" t="n">
+      <c r="D55" s="6">
         <v>1.75</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>44540</v>
       </c>
-      <c r="B56" s="6" t="n">
+      <c r="B56" s="6">
         <v>2</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>44541</v>
       </c>
-      <c r="B57" s="6" t="n">
+      <c r="B57" s="6">
         <v>2</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>44542</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="6" t="n">
+      <c r="D58" s="6">
         <v>2.5</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>44543</v>
       </c>
-      <c r="B59" s="6" t="n">
+      <c r="B59" s="6">
         <v>4</v>
       </c>
-      <c r="C59" s="6" t="n">
+      <c r="C59" s="6">
         <v>3</v>
       </c>
-      <c r="D59" s="6" t="n">
+      <c r="D59" s="6">
         <v>5.25</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>44544</v>
       </c>
-      <c r="B60" s="6" t="n">
+      <c r="B60" s="6">
         <v>4</v>
       </c>
-      <c r="C60" s="6" t="n">
+      <c r="C60" s="6">
         <v>4.5</v>
       </c>
-      <c r="D60" s="6" t="n">
+      <c r="D60" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>44545</v>
       </c>
-      <c r="B61" s="6" t="n">
+      <c r="B61" s="6">
         <v>3</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>44546</v>
       </c>
-      <c r="B62" s="6" t="n">
+      <c r="B62" s="6">
         <v>5</v>
       </c>
-      <c r="C62" s="6" t="n">
+      <c r="C62" s="6">
         <v>4</v>
       </c>
-      <c r="D62" s="6" t="n">
+      <c r="D62" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
         <v>44547</v>
       </c>
-      <c r="B63" s="6" t="n">
+      <c r="B63" s="6">
         <v>4</v>
       </c>
-      <c r="C63" s="6" t="n">
+      <c r="C63" s="6">
         <v>1.5</v>
       </c>
-      <c r="D63" s="6" t="n">
+      <c r="D63" s="6">
         <v>2.5</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
         <v>44548</v>
       </c>
-      <c r="B64" s="6" t="n">
+      <c r="B64" s="6">
         <v>2</v>
       </c>
       <c r="C64" s="6"/>
-      <c r="D64" s="6" t="n">
+      <c r="D64" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>44549</v>
       </c>
-      <c r="B65" s="6" t="n">
+      <c r="B65" s="6">
         <v>7</v>
       </c>
-      <c r="C65" s="6" t="n">
+      <c r="C65" s="6">
         <v>9</v>
       </c>
-      <c r="D65" s="6" t="n">
+      <c r="D65" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>44550</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>44551</v>
       </c>
-      <c r="B67" s="6"/>
+      <c r="B67" s="6">
+        <v>2</v>
+      </c>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>44552</v>
       </c>
-      <c r="B68" s="6"/>
+      <c r="B68" s="6">
+        <v>1</v>
+      </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>44553</v>
       </c>
-      <c r="B69" s="6"/>
+      <c r="B69" s="6">
+        <v>4</v>
+      </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>44554</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>44555</v>
       </c>
-      <c r="B71" s="6"/>
+      <c r="B71" s="6">
+        <v>2</v>
+      </c>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>44556</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>44557</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>44558</v>
       </c>
-      <c r="B74" s="6"/>
+      <c r="B74" s="6">
+        <v>2.5</v>
+      </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
         <v>44559</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
         <v>44560</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
         <v>44561</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
         <v>44562</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
         <v>44563</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
         <v>44564</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
         <v>44565</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
         <v>44566</v>
       </c>
-      <c r="B82" s="6"/>
+      <c r="B82" s="6">
+        <v>4</v>
+      </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
         <v>44567</v>
       </c>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
         <v>44568</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
         <v>44569</v>
       </c>
-      <c r="B85" s="6"/>
+      <c r="B85" s="6">
+        <v>2</v>
+      </c>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
         <v>44570</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="B86" s="6">
+        <v>4.5</v>
+      </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
         <v>44571</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
         <v>44572</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
         <v>44573</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
         <v>44574</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
         <v>44575</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
         <v>44576</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
         <v>44577</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
         <v>44578</v>
       </c>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
     </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
         <v>44579</v>
       </c>
-      <c r="B95" s="6"/>
+      <c r="B95" s="6">
+        <v>3</v>
+      </c>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
         <v>44580</v>
       </c>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
         <v>44581</v>
       </c>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
         <v>44582</v>
       </c>
-      <c r="B98" s="6"/>
+      <c r="B98" s="6">
+        <v>3.5</v>
+      </c>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
         <v>44583</v>
       </c>
-      <c r="B99" s="6"/>
+      <c r="B99" s="6">
+        <v>2.5</v>
+      </c>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
         <v>44584</v>
       </c>
-      <c r="B100" s="6"/>
+      <c r="B100" s="6">
+        <v>4</v>
+      </c>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
         <v>44585</v>
       </c>
       <c r="B101" s="6"/>
     </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
         <v>44586</v>
       </c>
-      <c r="B102" s="6"/>
-    </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="B102" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
         <v>44587</v>
       </c>
-      <c r="B103" s="6"/>
-    </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="B103" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
         <v>44588</v>
       </c>
-      <c r="B104" s="6"/>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="B104" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
         <v>44589</v>
       </c>
-      <c r="B105" s="6"/>
-    </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="B105" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
         <v>44590</v>
       </c>
-      <c r="B106" s="6"/>
-    </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="B106" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
         <v>44591</v>
       </c>
-      <c r="B107" s="6"/>
-    </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="B107" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
         <v>44592</v>
       </c>
       <c r="B108" s="6"/>
     </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
         <v>44593</v>
       </c>
       <c r="B109" s="6"/>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
         <v>44594</v>
       </c>
       <c r="B110" s="6"/>
     </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
         <v>44595</v>
       </c>
       <c r="B111" s="6"/>
     </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
         <v>44596</v>
       </c>
       <c r="B112" s="6"/>
     </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
         <v>44597</v>
       </c>
       <c r="B113" s="6"/>
     </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
         <v>44598</v>
       </c>
       <c r="B114" s="6"/>
     </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
         <v>44599</v>
       </c>
       <c r="B115" s="6"/>
     </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
         <v>44600</v>
       </c>
       <c r="B116" s="6"/>
     </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
         <v>44601</v>
       </c>
       <c r="B117" s="6"/>
     </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
         <v>44602</v>
       </c>
       <c r="B118" s="6"/>
     </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
         <v>44603</v>
       </c>
       <c r="B119" s="6"/>
     </row>
-    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
         <v>44604</v>
       </c>
       <c r="B120" s="6"/>
     </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
         <v>44605</v>
       </c>
       <c r="B121" s="6"/>
     </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
         <v>44606</v>
       </c>
       <c r="B122" s="6"/>
     </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
         <v>44607</v>
       </c>
       <c r="B123" s="6"/>
     </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
         <v>44608</v>
       </c>
       <c r="B124" s="6"/>
     </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
         <v>44609</v>
       </c>
       <c r="B125" s="6"/>
     </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
         <v>44610</v>
       </c>
       <c r="B126" s="6"/>
     </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
         <v>44611</v>
       </c>
       <c r="B127" s="6"/>
     </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
         <v>44612</v>
       </c>
       <c r="B128" s="6"/>
     </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
         <v>44613</v>
       </c>
       <c r="B129" s="6"/>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
         <v>44614</v>
       </c>
       <c r="B130" s="6"/>
     </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
         <v>44615</v>
       </c>
       <c r="B131" s="6"/>
     </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
         <v>44616</v>
       </c>
       <c r="B132" s="6"/>
     </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
         <v>44617</v>
       </c>
       <c r="B133" s="6"/>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
         <v>44618</v>
       </c>
       <c r="B134" s="6"/>
     </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
         <v>44619</v>
       </c>
       <c r="B135" s="6"/>
     </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
         <v>44620</v>
       </c>
       <c r="B136" s="6"/>
     </row>
-    <row r="138" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="B138" s="8" t="str">
-        <f aca="false">B2</f>
+        <f>B2</f>
         <v>Name</v>
       </c>
       <c r="C138" s="8" t="str">
-        <f aca="false">C2</f>
+        <f>C2</f>
         <v>Name</v>
       </c>
       <c r="D138" s="8" t="str">
-        <f aca="false">D2</f>
+        <f>D2</f>
         <v>Name</v>
       </c>
       <c r="F138" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B139" s="11" t="n">
-        <f aca="false">SUM(B5:B136)</f>
-        <v>48.4</v>
-      </c>
-      <c r="C139" s="11" t="n">
-        <f aca="false">SUM(C5:C136)</f>
+      <c r="B139" s="11">
+        <f>SUM(B5:B136)</f>
+        <v>101.4</v>
+      </c>
+      <c r="C139" s="11">
+        <f>SUM(C5:C136)</f>
         <v>33.5</v>
       </c>
-      <c r="D139" s="11" t="n">
-        <f aca="false">SUM(D5:D136)</f>
+      <c r="D139" s="11">
+        <f>SUM(D5:D136)</f>
         <v>42.5</v>
       </c>
       <c r="E139" s="11"/>
-      <c r="F139" s="11" t="n">
-        <f aca="false">SUM(B139:D139)</f>
-        <v>124.4</v>
+      <c r="F139" s="11">
+        <f>SUM(B139:D139)</f>
+        <v>177.4</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>

</xml_diff>